<commit_message>
updated html and combined into one file
</commit_message>
<xml_diff>
--- a/employees_spsi.xlsx
+++ b/employees_spsi.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft4941168-my.sharepoint.com/personal/jscheftic_spsi_com/Documents/Desktop/SPSI Code/SPSI Signatures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscheftic\SPSI Code\SPSI Signatures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{BC854909-11F9-4640-A7C5-417EF113CDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1386470C-AC7C-4C64-99A5-EBABE99B9281}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0468CFE8-3C39-46EC-B6F6-F57EAB1DB4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-13140" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +61,6 @@
     <t>Becky Tarbox</t>
   </si>
   <si>
-    <t>Brennan Lietzau</t>
-  </si>
-  <si>
     <t>Brett Mattys</t>
   </si>
   <si>
@@ -79,9 +79,6 @@
     <t>Ernesto Saenz</t>
   </si>
   <si>
-    <t>Jake Young</t>
-  </si>
-  <si>
     <t>Janet Clark</t>
   </si>
   <si>
@@ -115,36 +112,21 @@
     <t>Sandy Reopelle</t>
   </si>
   <si>
-    <t>Shari Hanson</t>
-  </si>
-  <si>
     <t>Skip Zuse</t>
   </si>
   <si>
-    <t>Steve Southard</t>
-  </si>
-  <si>
     <t>Tim Ricci</t>
   </si>
   <si>
     <t>Tom Schwab</t>
   </si>
   <si>
-    <t>Tony Bragg</t>
-  </si>
-  <si>
     <t>Val Martinez</t>
   </si>
   <si>
-    <t>Zach Young</t>
-  </si>
-  <si>
     <t>Ross Esenberg</t>
   </si>
   <si>
-    <t>Dustin Kacal</t>
-  </si>
-  <si>
     <t>Accounts Receivable</t>
   </si>
   <si>
@@ -160,9 +142,6 @@
     <t>Senior Controller</t>
   </si>
   <si>
-    <t>Service Technician &amp; Inside Support</t>
-  </si>
-  <si>
     <t>Customer Service</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
     <t>Operations Manager</t>
   </si>
   <si>
-    <t>Parts &amp; Service Manager</t>
-  </si>
-  <si>
     <t>Sales Support</t>
   </si>
   <si>
@@ -205,15 +181,9 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>Director, Sales &amp; Service</t>
   </si>
   <si>
-    <t>Outside Sales &amp; Service Technician</t>
-  </si>
-  <si>
     <t>763-391-7390</t>
   </si>
   <si>
@@ -238,9 +208,6 @@
     <t>1006</t>
   </si>
   <si>
-    <t>1019</t>
-  </si>
-  <si>
     <t>1011</t>
   </si>
   <si>
@@ -256,9 +223,6 @@
     <t>1065</t>
   </si>
   <si>
-    <t>1063</t>
-  </si>
-  <si>
     <t>1026</t>
   </si>
   <si>
@@ -283,9 +247,6 @@
     <t>1023</t>
   </si>
   <si>
-    <t>1344</t>
-  </si>
-  <si>
     <t>1014</t>
   </si>
   <si>
@@ -310,9 +271,6 @@
     <t>763-255-1006</t>
   </si>
   <si>
-    <t>763-255-1019</t>
-  </si>
-  <si>
     <t>763-255-1011</t>
   </si>
   <si>
@@ -364,24 +322,15 @@
     <t>513-257-4717</t>
   </si>
   <si>
-    <t>913-982-1344</t>
-  </si>
-  <si>
     <t>763-255-1014</t>
   </si>
   <si>
     <t>763-255-1010</t>
   </si>
   <si>
-    <t>515-491-5967</t>
-  </si>
-  <si>
     <t>763-255-1021</t>
   </si>
   <si>
-    <t>682-323-0063</t>
-  </si>
-  <si>
     <t>612-309-1660</t>
   </si>
   <si>
@@ -433,9 +382,6 @@
     <t>btarbox@spsi.com</t>
   </si>
   <si>
-    <t>blietzau@spsi.com</t>
-  </si>
-  <si>
     <t>bmattys@spsi.com</t>
   </si>
   <si>
@@ -454,9 +400,6 @@
     <t>esaenz@spsi.com</t>
   </si>
   <si>
-    <t>jyoung@spsi.com</t>
-  </si>
-  <si>
     <t>jclark@spsi.com</t>
   </si>
   <si>
@@ -496,30 +439,18 @@
     <t>szuse@spsi.com</t>
   </si>
   <si>
-    <t>ssouthard@spsi.com</t>
-  </si>
-  <si>
     <t>tricci@spsi.com</t>
   </si>
   <si>
     <t>tschwab@spsi.com</t>
   </si>
   <si>
-    <t>tbragg@spsi.com</t>
-  </si>
-  <si>
     <t>vmartinez@spsi.com</t>
   </si>
   <si>
-    <t>zyoung@spsi.com</t>
-  </si>
-  <si>
     <t>resenberg@spsi.com</t>
   </si>
   <si>
-    <t>dkacal@spsi.com</t>
-  </si>
-  <si>
     <t>mbunde@spsi.com</t>
   </si>
   <si>
@@ -527,13 +458,49 @@
   </si>
   <si>
     <t>tcodute@spsi.com</t>
+  </si>
+  <si>
+    <t>Shari Lynn Hanson</t>
+  </si>
+  <si>
+    <t>Colin Huggins</t>
+  </si>
+  <si>
+    <t>Chuggins@spsi.com</t>
+  </si>
+  <si>
+    <t>Kyle Jones</t>
+  </si>
+  <si>
+    <t>612-812-1699</t>
+  </si>
+  <si>
+    <t>kjones@spsi.com</t>
+  </si>
+  <si>
+    <t>Bryan Alvarez</t>
+  </si>
+  <si>
+    <t>913-624-4722</t>
+  </si>
+  <si>
+    <t>balvarez@spsi.com</t>
+  </si>
+  <si>
+    <t>Case Bartow</t>
+  </si>
+  <si>
+    <t>Service &amp; Parts Manager</t>
+  </si>
+  <si>
+    <t>Business System Solutions Integrator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,16 +536,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -601,12 +580,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC9C9C9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -617,6 +605,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -922,27 +913,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" customWidth="1"/>
-    <col min="6" max="6" width="31.36328125" customWidth="1"/>
-    <col min="7" max="7" width="21.54296875" customWidth="1"/>
-    <col min="8" max="8" width="28.1796875" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="30.08984375" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,13 +941,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -972,1115 +963,1049 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3">
         <v>1037</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="I7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" t="s">
-        <v>140</v>
+        <v>85</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>141</v>
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>123</v>
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="3"/>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="I14" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" t="s">
-        <v>148</v>
-      </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
         <v>131</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" t="s">
-        <v>166</v>
-      </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" t="s">
-        <v>150</v>
+        <v>93</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="I22" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="H23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>152</v>
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
+        <v>134</v>
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" t="s">
+        <v>138</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" t="s">
+        <v>139</v>
+      </c>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" t="s">
+        <v>140</v>
+      </c>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" t="s">
+        <v>141</v>
+      </c>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" t="s">
+        <v>105</v>
+      </c>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" t="s">
+        <v>106</v>
+      </c>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35">
+        <v>1008</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" t="s">
+        <v>152</v>
+      </c>
+      <c r="I36" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I25" t="s">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>154</v>
       </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" t="s">
-        <v>156</v>
-      </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" t="s">
-        <v>157</v>
-      </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I29" t="s">
-        <v>158</v>
-      </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="I30" t="s">
-        <v>159</v>
-      </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="I31" t="s">
-        <v>160</v>
-      </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" t="s">
-        <v>161</v>
-      </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I33" t="s">
-        <v>162</v>
-      </c>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" t="s">
-        <v>163</v>
-      </c>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I35" t="s">
-        <v>164</v>
-      </c>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I36" t="s">
-        <v>165</v>
-      </c>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="F37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" t="s">
-        <v>122</v>
-      </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" t="s">
-        <v>123</v>
-      </c>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" t="s">
-        <v>124</v>
-      </c>
-      <c r="J39" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="G37">
+        <v>1065</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I12" r:id="rId1" xr:uid="{95EA1AC7-1CC5-4FB9-B6E1-2FD3647E531E}"/>
+    <hyperlink ref="I11" r:id="rId1" xr:uid="{95EA1AC7-1CC5-4FB9-B6E1-2FD3647E531E}"/>
     <hyperlink ref="I3" r:id="rId2" xr:uid="{E3450331-AD92-4BBB-A22B-A16FDA8AEB64}"/>
-    <hyperlink ref="I23" r:id="rId3" xr:uid="{6AAED2F0-F8D8-4FF4-ACD1-C31F181977F0}"/>
-    <hyperlink ref="I26" r:id="rId4" xr:uid="{D0ADFA12-4299-465B-9A7F-9CAD2594F893}"/>
+    <hyperlink ref="I21" r:id="rId3" xr:uid="{6AAED2F0-F8D8-4FF4-ACD1-C31F181977F0}"/>
+    <hyperlink ref="I24" r:id="rId4" xr:uid="{D0ADFA12-4299-465B-9A7F-9CAD2594F893}"/>
     <hyperlink ref="I4" r:id="rId5" xr:uid="{D65B02A3-28F0-4EC6-A7A0-E462DF63F258}"/>
+    <hyperlink ref="I34" r:id="rId6" xr:uid="{44CB69C5-8668-4D15-9AC8-28BD0941640E}"/>
+    <hyperlink ref="I35" r:id="rId7" xr:uid="{455D0F10-5F93-4934-8480-A2ADB02ADB24}"/>
+    <hyperlink ref="I36" r:id="rId8" xr:uid="{809D9758-0FE4-4826-A9DB-D6860327E3A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update employee signatures and remove Tony Bragg's signature
- Added a border-bottom style to the signature tables for better separation.
- Updated job titles for Jay Milliren and Kyle Jones.
- Removed the celebration text from all signatures.
- Deleted the signature file for Tony Bragg.
- Updated the employees_spsi.xlsx file.
</commit_message>
<xml_diff>
--- a/employees_spsi.xlsx
+++ b/employees_spsi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jscheftic\SPSI Code\SPSI Signatures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0468CFE8-3C39-46EC-B6F6-F57EAB1DB4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AC1D53-AFDD-4197-8F1D-0B35140A6237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-13140" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="-14610" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -915,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>